<commit_message>
weitere Bauteile zugeordnet (Widerstände und Dioden)
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A150567E-3BD2-40B5-9D7B-6116EE73A589}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Speed_sensor" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="159">
   <si>
     <t>Source:</t>
   </si>
@@ -196,9 +196,6 @@
     <t>D5</t>
   </si>
   <si>
-    <t>Yellow (2V)</t>
-  </si>
-  <si>
     <t>H1</t>
   </si>
   <si>
@@ -454,16 +451,58 @@
     <t>C26087</t>
   </si>
   <si>
-    <t>verwende 270</t>
-  </si>
-  <si>
     <t>C310256</t>
+  </si>
+  <si>
+    <t>C294637</t>
+  </si>
+  <si>
+    <t>C25535</t>
+  </si>
+  <si>
+    <t>C140214</t>
+  </si>
+  <si>
+    <t>C304599</t>
+  </si>
+  <si>
+    <t>C25170</t>
+  </si>
+  <si>
+    <t>nein (nur 20)</t>
+  </si>
+  <si>
+    <t>C305012</t>
+  </si>
+  <si>
+    <t>C22857</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>verwende 10,7k</t>
+  </si>
+  <si>
+    <t>C205443</t>
+  </si>
+  <si>
+    <t>C205445</t>
+  </si>
+  <si>
+    <t>verwende 510</t>
+  </si>
+  <si>
+    <t>Orange-3V</t>
+  </si>
+  <si>
+    <t>C150464</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1315,20 +1354,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1377,13 +1417,13 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1537,7 +1577,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1551,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1565,7 +1605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1579,7 +1619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1593,7 +1633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1607,7 +1647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1621,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1635,7 +1675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1649,7 +1689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1663,7 +1703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1677,7 +1717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1691,7 +1731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1705,7 +1745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1719,7 +1759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1732,8 +1772,14 @@
       <c r="D30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>154</v>
+      </c>
+      <c r="G30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1746,8 +1792,14 @@
       <c r="D31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1760,13 +1812,19 @@
       <c r="D32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
         <v>49</v>
@@ -1774,479 +1832,557 @@
       <c r="D33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" t="s">
         <v>60</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>61</v>
       </c>
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>63</v>
       </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="C37" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-      <c r="C38" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" t="s">
         <v>71</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="D39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>77</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" t="s">
         <v>80</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="D43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" t="s">
         <v>86</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>87</v>
-      </c>
-      <c r="D44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>88</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>89</v>
       </c>
-      <c r="D45" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>91</v>
       </c>
-      <c r="C46" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" s="1">
+        <v>470</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" t="s">
+        <v>156</v>
+      </c>
+      <c r="F47" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="1">
-        <v>200</v>
-      </c>
-      <c r="C47" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" t="s">
-        <v>93</v>
-      </c>
       <c r="D48" t="s">
         <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49" t="s">
         <v>16</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
+      </c>
+      <c r="G49" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="1">
-        <v>510</v>
+        <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
+      </c>
+      <c r="F50" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="1">
         <v>270</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
+      </c>
+      <c r="F51" t="s">
+        <v>143</v>
+      </c>
+      <c r="G51" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" t="s">
         <v>101</v>
       </c>
-      <c r="C52" t="s">
-        <v>102</v>
-      </c>
       <c r="D52" t="s">
         <v>16</v>
+      </c>
+      <c r="F52" t="s">
+        <v>147</v>
+      </c>
+      <c r="G52" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
         <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>146</v>
+      </c>
+      <c r="G53" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
         <v>16</v>
+      </c>
+      <c r="F54" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D55" t="s">
         <v>16</v>
+      </c>
+      <c r="F55" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
         <v>16</v>
       </c>
       <c r="F56" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" t="s">
         <v>141</v>
-      </c>
-      <c r="G56" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="1">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D57" t="s">
         <v>16</v>
       </c>
-      <c r="E57" t="s">
-        <v>144</v>
-      </c>
       <c r="F57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" t="s">
         <v>113</v>
-      </c>
-      <c r="C59" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" t="s">
         <v>116</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>117</v>
       </c>
-      <c r="D60" t="s">
-        <v>118</v>
+      <c r="G60" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" t="s">
         <v>120</v>
       </c>
-      <c r="C61" t="s">
-        <v>121</v>
+      <c r="G61" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" t="s">
         <v>123</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>124</v>
       </c>
-      <c r="D62" t="s">
-        <v>125</v>
+      <c r="G62" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" t="s">
         <v>127</v>
-      </c>
-      <c r="C63" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" t="s">
         <v>130</v>
       </c>
-      <c r="C64" t="s">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B65" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" t="s">
         <v>133</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>134</v>
       </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" t="s">
         <v>136</v>
       </c>
-      <c r="C66" t="s">
-        <v>137</v>
-      </c>
       <c r="D66" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated footprint L1, BOM erweitert und weitere Teile zugeordnet
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A150567E-3BD2-40B5-9D7B-6116EE73A589}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1428B881-7F18-4FFC-BC00-EC882D1D9AA6}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="165">
   <si>
     <t>Source:</t>
   </si>
@@ -469,9 +469,6 @@
     <t>C25170</t>
   </si>
   <si>
-    <t>nein (nur 20)</t>
-  </si>
-  <si>
     <t>C305012</t>
   </si>
   <si>
@@ -497,13 +494,34 @@
   </si>
   <si>
     <t>C150464</t>
+  </si>
+  <si>
+    <t>Free Sample (5x)</t>
+  </si>
+  <si>
+    <t>C81080</t>
+  </si>
+  <si>
+    <t>C110926</t>
+  </si>
+  <si>
+    <t>C248711</t>
+  </si>
+  <si>
+    <t>ja (nur 20)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>C165948</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,6 +656,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -945,7 +971,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -988,8 +1014,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1000,8 +1027,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1032,6 +1060,7 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1357,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,6 +1465,9 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
+      <c r="G6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1744,6 +1776,9 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
+      <c r="G28" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1758,6 +1793,12 @@
       <c r="D29" t="s">
         <v>16</v>
       </c>
+      <c r="F29" t="s">
+        <v>153</v>
+      </c>
+      <c r="G29" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1773,7 +1814,7 @@
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G30" t="s">
         <v>141</v>
@@ -1793,7 +1834,7 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G31" t="s">
         <v>141</v>
@@ -1813,7 +1854,7 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G32" t="s">
         <v>141</v>
@@ -1824,7 +1865,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" t="s">
         <v>49</v>
@@ -1833,7 +1874,7 @@
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G33" t="s">
         <v>141</v>
@@ -1852,6 +1893,9 @@
       <c r="D34" t="s">
         <v>16</v>
       </c>
+      <c r="G34" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1866,6 +1910,9 @@
       <c r="D35" t="s">
         <v>16</v>
       </c>
+      <c r="G35" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1880,6 +1927,9 @@
       <c r="D36" t="s">
         <v>16</v>
       </c>
+      <c r="G36" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1894,6 +1944,9 @@
       <c r="D37" t="s">
         <v>16</v>
       </c>
+      <c r="G37" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1908,6 +1961,9 @@
       <c r="D38" t="s">
         <v>16</v>
       </c>
+      <c r="G38" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1922,6 +1978,9 @@
       <c r="D39" t="s">
         <v>16</v>
       </c>
+      <c r="G39" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1936,6 +1995,9 @@
       <c r="D40" t="s">
         <v>16</v>
       </c>
+      <c r="G40" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1947,8 +2009,14 @@
       <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="6" t="s">
         <v>77</v>
+      </c>
+      <c r="F41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2035,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F47" t="s">
         <v>148</v>
@@ -2058,13 +2126,13 @@
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F48" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" t="s">
         <v>151</v>
-      </c>
-      <c r="G48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2081,10 +2149,10 @@
         <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G49" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2277,6 +2345,12 @@
       <c r="C59" t="s">
         <v>113</v>
       </c>
+      <c r="F59" t="s">
+        <v>159</v>
+      </c>
+      <c r="G59" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -2305,8 +2379,11 @@
       <c r="C61" t="s">
         <v>120</v>
       </c>
+      <c r="E61" t="s">
+        <v>158</v>
+      </c>
       <c r="G61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2336,6 +2413,12 @@
       <c r="C63" t="s">
         <v>127</v>
       </c>
+      <c r="F63" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -2347,6 +2430,12 @@
       <c r="C64" t="s">
         <v>130</v>
       </c>
+      <c r="F64" t="s">
+        <v>161</v>
+      </c>
+      <c r="G64" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -2386,7 +2475,10 @@
       <c r="B67" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D41" r:id="rId1" xr:uid="{7BE6B800-FCF7-4D11-B03B-80E349998BE8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
im layout paar Bezeichnungen entfernt (die zurück gekommen sind nachdem footprints geändert wurden)
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1428B881-7F18-4FFC-BC00-EC882D1D9AA6}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6EAA89FC-E4D5-4986-B40B-7B3E017779F7}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,9 +271,6 @@
     <t>2,2u</t>
   </si>
   <si>
-    <t>Resistor_SMD:R_0805_2012Metric_Pad1.20x1.40mm_HandSolder</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -515,6 +512,9 @@
   </si>
   <si>
     <t>C165948</t>
+  </si>
+  <si>
+    <t>Inductor_SMD:L_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
   </si>
 </sst>
 </file>
@@ -1446,13 +1446,13 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,7 +1777,7 @@
         <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1794,10 +1794,10 @@
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1814,10 +1814,10 @@
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1834,10 +1834,10 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1854,10 +1854,10 @@
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1865,7 +1865,7 @@
         <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
         <v>49</v>
@@ -1874,10 +1874,10 @@
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>16</v>
       </c>
       <c r="G35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
         <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
         <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
         <v>16</v>
       </c>
       <c r="G39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1996,7 +1996,7 @@
         <v>16</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2013,10 +2013,10 @@
         <v>77</v>
       </c>
       <c r="F41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2041,7 +2041,7 @@
         <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
@@ -2049,13 +2049,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" t="s">
         <v>85</v>
-      </c>
-      <c r="C44" t="s">
-        <v>86</v>
       </c>
       <c r="D44" t="s">
         <v>16</v>
@@ -2063,13 +2063,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
         <v>16</v>
@@ -2091,384 +2091,384 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="1">
         <v>470</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" t="s">
         <v>150</v>
-      </c>
-      <c r="G48" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" t="s">
         <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="1">
         <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" s="1">
         <v>270</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" t="s">
         <v>100</v>
       </c>
-      <c r="C52" t="s">
-        <v>101</v>
-      </c>
       <c r="D52" t="s">
         <v>16</v>
       </c>
       <c r="F52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
         <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
         <v>16</v>
       </c>
       <c r="F54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
         <v>16</v>
       </c>
       <c r="F55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
         <v>16</v>
       </c>
       <c r="F56" t="s">
+        <v>139</v>
+      </c>
+      <c r="G56" t="s">
         <v>140</v>
-      </c>
-      <c r="G56" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="1">
         <v>270</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s">
         <v>16</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
         <v>16</v>
       </c>
       <c r="F58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" t="s">
         <v>112</v>
       </c>
-      <c r="C59" t="s">
-        <v>113</v>
-      </c>
       <c r="F59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" t="s">
         <v>115</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>116</v>
       </c>
-      <c r="D60" t="s">
-        <v>117</v>
-      </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" t="s">
         <v>119</v>
       </c>
-      <c r="C61" t="s">
-        <v>120</v>
-      </c>
       <c r="E61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" t="s">
         <v>122</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>123</v>
       </c>
-      <c r="D62" t="s">
-        <v>124</v>
-      </c>
       <c r="G62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" t="s">
         <v>126</v>
       </c>
-      <c r="C63" t="s">
-        <v>127</v>
-      </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" t="s">
         <v>129</v>
       </c>
-      <c r="C64" t="s">
-        <v>130</v>
-      </c>
       <c r="F64" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" t="s">
         <v>132</v>
       </c>
-      <c r="C65" t="s">
-        <v>133</v>
-      </c>
       <c r="D65" t="s">
         <v>16</v>
       </c>
       <c r="G65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" t="s">
         <v>135</v>
       </c>
-      <c r="C66" t="s">
-        <v>136</v>
-      </c>
       <c r="D66" t="s">
         <v>16</v>
       </c>
       <c r="G66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
restliche Bauteile zugeornet und raus gesucht (bei LCSC bereit zum Bestellen); restliche Markierungen im Layout gemacht; 4 Kerben an langen Seiten des PCB hinzugefügt um ggf. PCB in Gehäuse zu drücken (a la Pressfit)
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6EAA89FC-E4D5-4986-B40B-7B3E017779F7}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0F842455-668E-48C1-A9DD-D2B531F4BD6D}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Speed_sensor" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="178">
   <si>
     <t>Source:</t>
   </si>
@@ -515,13 +515,52 @@
   </si>
   <si>
     <t>Inductor_SMD:L_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
+  </si>
+  <si>
+    <t>C92487</t>
+  </si>
+  <si>
+    <t>C392963</t>
+  </si>
+  <si>
+    <t>ja, aber trotzdem bestellen</t>
+  </si>
+  <si>
+    <t>C1592</t>
+  </si>
+  <si>
+    <t>C19666</t>
+  </si>
+  <si>
+    <t>C696853</t>
+  </si>
+  <si>
+    <t>C26406</t>
+  </si>
+  <si>
+    <t>C40459</t>
+  </si>
+  <si>
+    <t>C258500</t>
+  </si>
+  <si>
+    <t>C90196</t>
+  </si>
+  <si>
+    <t>C1035</t>
+  </si>
+  <si>
+    <t>C329619</t>
+  </si>
+  <si>
+    <t>C95973</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +702,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1016,7 +1061,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1028,6 +1073,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1387,20 +1433,20 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="1" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1416,7 +1462,7 @@
         <v>44328.924131944441</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1478,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1501,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +1515,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1482,8 +1528,14 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1496,8 +1548,14 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1505,13 +1563,19 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1524,8 +1588,14 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1538,8 +1608,14 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1552,8 +1628,14 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1566,8 +1648,14 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1580,8 +1668,14 @@
       <c r="D14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1594,8 +1688,14 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1608,8 +1708,14 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1622,8 +1728,14 @@
       <c r="D17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1636,8 +1748,11 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1650,8 +1765,14 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1664,8 +1785,14 @@
       <c r="D20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1678,8 +1805,14 @@
       <c r="D21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1692,8 +1825,14 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1706,8 +1845,14 @@
       <c r="D23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1720,8 +1865,14 @@
       <c r="D24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1734,8 +1885,14 @@
       <c r="D25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1748,8 +1905,14 @@
       <c r="D26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1762,8 +1925,14 @@
       <c r="D27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1780,7 +1949,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1800,7 +1969,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1820,7 +1989,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1840,7 +2009,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1860,7 +2029,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -1880,7 +2049,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1897,7 +2066,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1914,7 +2083,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1931,7 +2100,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -1948,7 +2117,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1965,7 +2134,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -1982,7 +2151,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1999,7 +2168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -2019,7 +2188,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2033,7 +2202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2046,8 +2215,14 @@
       <c r="D43" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -2060,8 +2235,14 @@
       <c r="D44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F44" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2074,8 +2255,14 @@
       <c r="D45" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2088,8 +2275,14 @@
       <c r="D46" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2112,7 +2305,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2135,7 +2328,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2155,7 +2348,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2175,7 +2368,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -2195,7 +2388,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -2215,7 +2408,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2235,7 +2428,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2255,7 +2448,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -2275,7 +2468,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -2295,7 +2488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -2315,7 +2508,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2335,7 +2528,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2352,7 +2545,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2369,7 +2562,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -2386,7 +2579,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2403,7 +2596,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2420,7 +2613,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -2437,7 +2630,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>130</v>
       </c>
@@ -2454,7 +2647,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -2471,7 +2664,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
erste Bestellung bei LCSC gemacht (siehe excel-tabelle)
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0F842455-668E-48C1-A9DD-D2B531F4BD6D}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C8B56BE4-8840-4329-8FBA-14CB9E0580CC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Speed_sensor" sheetId="1" r:id="rId1"/>
@@ -517,9 +517,6 @@
     <t>Inductor_SMD:L_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
   </si>
   <si>
-    <t>C92487</t>
-  </si>
-  <si>
     <t>C392963</t>
   </si>
   <si>
@@ -554,6 +551,9 @@
   </si>
   <si>
     <t>C95973</t>
+  </si>
+  <si>
+    <t>C319196</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -888,6 +888,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1061,7 +1073,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1073,7 +1085,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1432,16 +1446,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" customWidth="1"/>
     <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
@@ -1529,7 +1544,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" t="s">
         <v>150</v>
@@ -1549,7 +1564,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G8" t="s">
         <v>150</v>
@@ -1568,11 +1583,11 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s">
         <v>166</v>
-      </c>
-      <c r="G9" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1588,8 +1603,8 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
-        <v>165</v>
+      <c r="F10" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="G10" t="s">
         <v>150</v>
@@ -1608,11 +1623,11 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" t="s">
         <v>166</v>
-      </c>
-      <c r="G11" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1628,8 +1643,8 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="s">
-        <v>165</v>
+      <c r="F12" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="G12" t="s">
         <v>150</v>
@@ -1648,8 +1663,8 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
-        <v>165</v>
+      <c r="F13" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="G13" t="s">
         <v>150</v>
@@ -1669,7 +1684,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" t="s">
         <v>150</v>
@@ -1688,11 +1703,11 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" t="s">
         <v>166</v>
-      </c>
-      <c r="G15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1708,11 +1723,11 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" t="s">
         <v>166</v>
-      </c>
-      <c r="G16" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1728,8 +1743,8 @@
       <c r="D17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
-        <v>170</v>
+      <c r="F17" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="G17" t="s">
         <v>140</v>
@@ -1765,11 +1780,11 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" t="s">
         <v>166</v>
-      </c>
-      <c r="G19" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1786,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G20" t="s">
         <v>150</v>
@@ -1806,7 +1821,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -1826,7 +1841,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G22" t="s">
         <v>150</v>
@@ -1845,8 +1860,8 @@
       <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
-        <v>172</v>
+      <c r="F23" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="G23" t="s">
         <v>140</v>
@@ -1866,7 +1881,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G24" t="s">
         <v>150</v>
@@ -1886,7 +1901,7 @@
         <v>16</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G25" t="s">
         <v>150</v>
@@ -1905,11 +1920,11 @@
       <c r="D26" t="s">
         <v>16</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" t="s">
         <v>166</v>
-      </c>
-      <c r="G26" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1925,8 +1940,8 @@
       <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="F27" t="s">
-        <v>165</v>
+      <c r="F27" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="G27" t="s">
         <v>150</v>
@@ -1962,7 +1977,7 @@
       <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G29" t="s">
@@ -1982,7 +1997,7 @@
       <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G30" t="s">
@@ -2002,7 +2017,7 @@
       <c r="D31" t="s">
         <v>16</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G31" t="s">
@@ -2022,7 +2037,7 @@
       <c r="D32" t="s">
         <v>16</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="9" t="s">
         <v>156</v>
       </c>
       <c r="G32" t="s">
@@ -2042,7 +2057,7 @@
       <c r="D33" t="s">
         <v>16</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G33" t="s">
@@ -2181,7 +2196,7 @@
       <c r="D41" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="8" t="s">
         <v>163</v>
       </c>
       <c r="G41" t="s">
@@ -2216,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G43" t="s">
         <v>150</v>
@@ -2236,7 +2251,7 @@
         <v>16</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G44" t="s">
         <v>150</v>
@@ -2256,7 +2271,7 @@
         <v>16</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G45" t="s">
         <v>150</v>
@@ -2275,8 +2290,8 @@
       <c r="D46" t="s">
         <v>16</v>
       </c>
-      <c r="F46" t="s">
-        <v>174</v>
+      <c r="F46" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="G46" t="s">
         <v>140</v>
@@ -2298,7 +2313,7 @@
       <c r="E47" t="s">
         <v>154</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="9" t="s">
         <v>147</v>
       </c>
       <c r="G47" t="s">
@@ -2321,7 +2336,7 @@
       <c r="E48" t="s">
         <v>151</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="8" t="s">
         <v>149</v>
       </c>
       <c r="G48" t="s">
@@ -2341,7 +2356,7 @@
       <c r="D49" t="s">
         <v>16</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="8" t="s">
         <v>148</v>
       </c>
       <c r="G49" t="s">
@@ -2361,7 +2376,7 @@
       <c r="D50" t="s">
         <v>16</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="9" t="s">
         <v>142</v>
       </c>
       <c r="G50" t="s">
@@ -2381,7 +2396,7 @@
       <c r="D51" t="s">
         <v>16</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="9" t="s">
         <v>142</v>
       </c>
       <c r="G51" t="s">
@@ -2401,7 +2416,7 @@
       <c r="D52" t="s">
         <v>16</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="9" t="s">
         <v>146</v>
       </c>
       <c r="G52" t="s">
@@ -2421,7 +2436,7 @@
       <c r="D53" t="s">
         <v>16</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G53" t="s">
@@ -2441,7 +2456,7 @@
       <c r="D54" t="s">
         <v>16</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="9" t="s">
         <v>144</v>
       </c>
       <c r="G54" t="s">
@@ -2461,7 +2476,7 @@
       <c r="D55" t="s">
         <v>16</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="9" t="s">
         <v>143</v>
       </c>
       <c r="G55" t="s">
@@ -2481,7 +2496,7 @@
       <c r="D56" t="s">
         <v>16</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="9" t="s">
         <v>139</v>
       </c>
       <c r="G56" t="s">
@@ -2501,7 +2516,7 @@
       <c r="D57" t="s">
         <v>16</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="9" t="s">
         <v>142</v>
       </c>
       <c r="G57" t="s">
@@ -2521,7 +2536,7 @@
       <c r="D58" t="s">
         <v>16</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="9" t="s">
         <v>141</v>
       </c>
       <c r="G58" t="s">
@@ -2538,7 +2553,7 @@
       <c r="C59" t="s">
         <v>112</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="9" t="s">
         <v>158</v>
       </c>
       <c r="G59" t="s">
@@ -2558,6 +2573,7 @@
       <c r="D60" t="s">
         <v>116</v>
       </c>
+      <c r="F60" s="9"/>
       <c r="G60" t="s">
         <v>140</v>
       </c>
@@ -2572,7 +2588,7 @@
       <c r="C61" t="s">
         <v>119</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G61" t="s">
@@ -2592,6 +2608,7 @@
       <c r="D62" t="s">
         <v>123</v>
       </c>
+      <c r="F62" s="9"/>
       <c r="G62" t="s">
         <v>140</v>
       </c>
@@ -2606,7 +2623,7 @@
       <c r="C63" t="s">
         <v>126</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="9" t="s">
         <v>159</v>
       </c>
       <c r="G63" t="s">
@@ -2623,7 +2640,7 @@
       <c r="C64" t="s">
         <v>129</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="9" t="s">
         <v>160</v>
       </c>
       <c r="G64" t="s">
@@ -2643,6 +2660,7 @@
       <c r="D65" t="s">
         <v>16</v>
       </c>
+      <c r="F65" s="9"/>
       <c r="G65" t="s">
         <v>140</v>
       </c>
@@ -2660,6 +2678,7 @@
       <c r="D66" t="s">
         <v>16</v>
       </c>
+      <c r="F66" s="9"/>
       <c r="G66" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
BOM tabelle nach erster Bestückung
</commit_message>
<xml_diff>
--- a/KiCad/Speed_sensor_BOM_custom.xlsx
+++ b/KiCad/Speed_sensor_BOM_custom.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4551c9f81874734a/Documents/Projekte/Speed_sensor/speed_sensor/KiCad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\Projekte\speed_sensor\KiCad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:40009_{D5DBD20E-9CD1-4C53-9318-6E7622FAAB02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C8B56BE4-8840-4329-8FBA-14CB9E0580CC}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="2664" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Speed_sensor" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="179">
   <si>
     <t>Source:</t>
   </si>
@@ -554,12 +553,15 @@
   </si>
   <si>
     <t>C319196</t>
+  </si>
+  <si>
+    <t>Bestückung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -710,7 +712,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,6 +901,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,7 +1093,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1088,6 +1108,9 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1443,25 +1466,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="54.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="94.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1477,7 +1501,7 @@
         <v>44328.924131944441</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1517,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1504,19 +1528,22 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1526,11 +1553,15 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1540,17 +1571,20 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="12">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1560,17 +1594,20 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="12">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1580,17 +1617,20 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="D9" s="12">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1600,17 +1640,20 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="12">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1620,17 +1663,20 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="D11" s="12">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1640,17 +1686,20 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="12">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1660,17 +1709,20 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="12">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1680,17 +1732,20 @@
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="D14" s="12">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1700,17 +1755,20 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1720,17 +1778,20 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1740,17 +1801,20 @@
       <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="D17" s="12">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1760,14 +1824,14 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1777,17 +1841,20 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="D19" s="12">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1797,17 +1864,20 @@
       <c r="C20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="12">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1817,17 +1887,20 @@
       <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1837,17 +1910,20 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1857,17 +1933,20 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="D23" s="12">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1877,17 +1956,20 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="D24" s="12">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1897,17 +1979,20 @@
       <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="D25" s="12">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1917,17 +2002,20 @@
       <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="D26" s="12">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1937,17 +2025,20 @@
       <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="7" t="s">
+      <c r="D27" s="12">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1957,14 +2048,14 @@
       <c r="C28" t="s">
         <v>23</v>
       </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1974,17 +2065,18 @@
       <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="9" t="s">
+      <c r="D29" s="12"/>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1994,17 +2086,18 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-      <c r="D30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="9" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -2014,17 +2107,18 @@
       <c r="C31" t="s">
         <v>49</v>
       </c>
-      <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="9" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -2034,17 +2128,18 @@
       <c r="C32" t="s">
         <v>56</v>
       </c>
-      <c r="D32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="9" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -2054,17 +2149,18 @@
       <c r="C33" t="s">
         <v>49</v>
       </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="9" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2074,14 +2170,14 @@
       <c r="C34" t="s">
         <v>60</v>
       </c>
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -2091,14 +2187,14 @@
       <c r="C35" t="s">
         <v>60</v>
       </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -2108,14 +2204,14 @@
       <c r="C36" t="s">
         <v>60</v>
       </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2125,14 +2221,14 @@
       <c r="C37" t="s">
         <v>60</v>
       </c>
-      <c r="D37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -2142,14 +2238,14 @@
       <c r="C38" t="s">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -2159,14 +2255,14 @@
       <c r="C39" t="s">
         <v>71</v>
       </c>
-      <c r="D39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2176,14 +2272,14 @@
       <c r="C40" t="s">
         <v>71</v>
       </c>
-      <c r="D40" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -2193,17 +2289,18 @@
       <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="12"/>
+      <c r="E41" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -2213,11 +2310,12 @@
       <c r="C42" t="s">
         <v>80</v>
       </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="10"/>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2227,17 +2325,20 @@
       <c r="C43" t="s">
         <v>164</v>
       </c>
-      <c r="D43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="7" t="s">
+      <c r="D43" s="12">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -2247,17 +2348,20 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="D44" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="7" t="s">
+      <c r="D44" s="12">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2267,17 +2371,20 @@
       <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="D45" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="D45" s="12">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2287,17 +2394,20 @@
       <c r="C46" t="s">
         <v>85</v>
       </c>
-      <c r="D46" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="9" t="s">
+      <c r="D46" s="12">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2307,20 +2417,23 @@
       <c r="C47" t="s">
         <v>100</v>
       </c>
-      <c r="D47" t="s">
-        <v>16</v>
+      <c r="D47" s="12">
+        <v>8</v>
       </c>
       <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="s">
         <v>154</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2330,20 +2443,23 @@
       <c r="C48" t="s">
         <v>91</v>
       </c>
-      <c r="D48" t="s">
-        <v>16</v>
+      <c r="D48" s="12">
+        <v>20</v>
       </c>
       <c r="E48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" t="s">
         <v>151</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="G48" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2353,17 +2469,20 @@
       <c r="C49" t="s">
         <v>91</v>
       </c>
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="8" t="s">
+      <c r="D49" s="12">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2373,17 +2492,20 @@
       <c r="C50" t="s">
         <v>100</v>
       </c>
-      <c r="D50" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="9" t="s">
+      <c r="D50" s="12">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -2393,17 +2515,20 @@
       <c r="C51" t="s">
         <v>100</v>
       </c>
-      <c r="D51" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="9" t="s">
+      <c r="D51" s="12">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -2413,17 +2538,20 @@
       <c r="C52" t="s">
         <v>100</v>
       </c>
-      <c r="D52" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="9" t="s">
+      <c r="D52" s="12">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -2433,17 +2561,20 @@
       <c r="C53" t="s">
         <v>100</v>
       </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" s="9" t="s">
+      <c r="D53" s="12">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2453,17 +2584,20 @@
       <c r="C54" t="s">
         <v>100</v>
       </c>
-      <c r="D54" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="9" t="s">
+      <c r="D54" s="12">
+        <v>12</v>
+      </c>
+      <c r="E54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -2473,17 +2607,20 @@
       <c r="C55" t="s">
         <v>100</v>
       </c>
-      <c r="D55" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" s="9" t="s">
+      <c r="D55" s="12">
+        <v>13</v>
+      </c>
+      <c r="E55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>106</v>
       </c>
@@ -2493,17 +2630,20 @@
       <c r="C56" t="s">
         <v>100</v>
       </c>
-      <c r="D56" t="s">
-        <v>16</v>
-      </c>
-      <c r="F56" s="9" t="s">
+      <c r="D56" s="12">
+        <v>14</v>
+      </c>
+      <c r="E56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -2513,17 +2653,20 @@
       <c r="C57" t="s">
         <v>100</v>
       </c>
-      <c r="D57" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="9" t="s">
+      <c r="D57" s="12">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2533,17 +2676,20 @@
       <c r="C58" t="s">
         <v>100</v>
       </c>
-      <c r="D58" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" s="9" t="s">
+      <c r="D58" s="12">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2553,14 +2699,15 @@
       <c r="C59" t="s">
         <v>112</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="D59" s="12"/>
+      <c r="G59" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2570,15 +2717,16 @@
       <c r="C60" t="s">
         <v>115</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="11"/>
+      <c r="E60" t="s">
         <v>116</v>
       </c>
-      <c r="F60" s="9"/>
-      <c r="G60" t="s">
+      <c r="G60" s="9"/>
+      <c r="H60" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -2588,14 +2736,15 @@
       <c r="C61" t="s">
         <v>119</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="D61" s="12"/>
+      <c r="F61" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2605,15 +2754,16 @@
       <c r="C62" t="s">
         <v>122</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="12"/>
+      <c r="E62" t="s">
         <v>123</v>
       </c>
-      <c r="F62" s="9"/>
-      <c r="G62" t="s">
+      <c r="G62" s="9"/>
+      <c r="H62" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2623,14 +2773,15 @@
       <c r="C63" t="s">
         <v>126</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="D63" s="12"/>
+      <c r="G63" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -2640,14 +2791,15 @@
       <c r="C64" t="s">
         <v>129</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="D64" s="12"/>
+      <c r="G64" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>130</v>
       </c>
@@ -2657,15 +2809,16 @@
       <c r="C65" t="s">
         <v>132</v>
       </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-      <c r="F65" s="9"/>
-      <c r="G65" t="s">
+      <c r="D65" s="12"/>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="9"/>
+      <c r="H65" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -2675,20 +2828,21 @@
       <c r="C66" t="s">
         <v>135</v>
       </c>
-      <c r="D66" t="s">
-        <v>16</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" t="s">
+      <c r="D66" s="12"/>
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="9"/>
+      <c r="H66" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D41" r:id="rId1" xr:uid="{7BE6B800-FCF7-4D11-B03B-80E349998BE8}"/>
+    <hyperlink ref="E41" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>